<commit_message>
tweaking slow reveal graphs to specifications
</commit_message>
<xml_diff>
--- a/Original Plot Work/Womans Suffrage Timeline/Data/data5.xlsx
+++ b/Original Plot Work/Womans Suffrage Timeline/Data/data5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RBY11\Documents\R_Work\Slow_Reveal_Graphs\Original Plot Work\Womans Suffrage Timeline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RBY11\Documents\R_work\Slow_Reveal_Graphs\Original Plot Work\Womans Suffrage Timeline\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F529E651-8E7B-419A-9382-F990D6503BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDDCDDB-B6F9-4422-AC08-5D748B496D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{A2B69022-1D9E-493D-ABC5-004A2EBF399C}"/>
+    <workbookView xWindow="4815" yWindow="1185" windowWidth="21600" windowHeight="11385" xr2:uid="{A2B69022-1D9E-493D-ABC5-004A2EBF399C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -771,7 +771,7 @@
   <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>